<commit_message>
update to metaphlan3 launcher script
</commit_message>
<xml_diff>
--- a/Rdata/OSF_analysis/sample_summary.xlsx
+++ b/Rdata/OSF_analysis/sample_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\microbial\Rdata\OSF_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6739818-08E3-42F0-987C-91BE5EB9C1A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5FAD20-634D-4C75-A6B6-6562266A78B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="38700" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2850" yWindow="2850" windowWidth="21600" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clinical data summary" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16080" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16080" uniqueCount="759">
   <si>
     <t>sample_type</t>
   </si>
@@ -2507,6 +2507,51 @@
   </si>
   <si>
     <t>Unknown</t>
+  </si>
+  <si>
+    <t>China:Shenzhen</t>
+  </si>
+  <si>
+    <t>China:Beijing</t>
+  </si>
+  <si>
+    <t>China:Xian</t>
+  </si>
+  <si>
+    <t>2018-01-02</t>
+  </si>
+  <si>
+    <t>2018-02-28</t>
+  </si>
+  <si>
+    <t>2018-02-08</t>
+  </si>
+  <si>
+    <t>2018-02-07</t>
+  </si>
+  <si>
+    <t>2016-04-18</t>
+  </si>
+  <si>
+    <t>2015-03-01</t>
+  </si>
+  <si>
+    <t>2018-03-30</t>
+  </si>
+  <si>
+    <t>2017-12-19</t>
+  </si>
+  <si>
+    <t>2017-10-31</t>
+  </si>
+  <si>
+    <t>2017-11-01</t>
+  </si>
+  <si>
+    <t>2018-05-03</t>
+  </si>
+  <si>
+    <t>2019-12-30</t>
   </si>
 </sst>
 </file>
@@ -2720,7 +2765,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3004,6 +3049,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3389,9 +3437,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMM227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BD1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BQ77" sqref="BQ77"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3421,7 +3469,7 @@
     <col min="66" max="66" width="99" style="4" customWidth="1"/>
     <col min="67" max="67" width="16.28515625" style="4" customWidth="1"/>
     <col min="68" max="68" width="16.28515625" style="1" customWidth="1"/>
-    <col min="69" max="69" width="24.85546875" style="1" customWidth="1"/>
+    <col min="69" max="69" width="16.85546875" style="1" customWidth="1"/>
     <col min="70" max="70" width="30.28515625" style="1" customWidth="1"/>
     <col min="71" max="71" width="20.85546875" style="1" customWidth="1"/>
     <col min="72" max="1010" width="8.7109375" style="1"/>
@@ -26553,8 +26601,8 @@
       <c r="BK100" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL100" s="16" t="s">
-        <v>130</v>
+      <c r="BL100" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM100" s="16">
         <v>43916</v>
@@ -26565,8 +26613,8 @@
       <c r="BO100" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP100" s="14" t="s">
-        <v>130</v>
+      <c r="BP100" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ100" s="14" t="s">
         <v>377</v>
@@ -26785,8 +26833,8 @@
       <c r="BK101" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL101" s="16" t="s">
-        <v>130</v>
+      <c r="BL101" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM101" s="16">
         <v>43916</v>
@@ -26797,8 +26845,8 @@
       <c r="BO101" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP101" s="14" t="s">
-        <v>130</v>
+      <c r="BP101" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ101" s="14" t="s">
         <v>377</v>
@@ -27017,8 +27065,8 @@
       <c r="BK102" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL102" s="65" t="s">
-        <v>130</v>
+      <c r="BL102" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM102" s="16">
         <v>43916</v>
@@ -27029,8 +27077,8 @@
       <c r="BO102" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP102" s="1" t="s">
-        <v>130</v>
+      <c r="BP102" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ102" s="14" t="s">
         <v>377</v>
@@ -27249,8 +27297,8 @@
       <c r="BK103" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL103" s="65" t="s">
-        <v>130</v>
+      <c r="BL103" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM103" s="16">
         <v>43916</v>
@@ -27261,8 +27309,8 @@
       <c r="BO103" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP103" s="1" t="s">
-        <v>130</v>
+      <c r="BP103" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ103" s="14" t="s">
         <v>377</v>
@@ -27481,8 +27529,8 @@
       <c r="BK104" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL104" s="65" t="s">
-        <v>130</v>
+      <c r="BL104" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM104" s="16">
         <v>43916</v>
@@ -27493,8 +27541,8 @@
       <c r="BO104" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP104" s="1" t="s">
-        <v>130</v>
+      <c r="BP104" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ104" s="14" t="s">
         <v>377</v>
@@ -27713,8 +27761,8 @@
       <c r="BK105" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL105" s="65" t="s">
-        <v>130</v>
+      <c r="BL105" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM105" s="16">
         <v>43916</v>
@@ -27725,8 +27773,8 @@
       <c r="BO105" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP105" s="1" t="s">
-        <v>130</v>
+      <c r="BP105" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ105" s="14" t="s">
         <v>377</v>
@@ -27945,8 +27993,8 @@
       <c r="BK106" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL106" s="65" t="s">
-        <v>130</v>
+      <c r="BL106" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM106" s="16">
         <v>43916</v>
@@ -27957,8 +28005,8 @@
       <c r="BO106" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP106" s="1" t="s">
-        <v>130</v>
+      <c r="BP106" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ106" s="14" t="s">
         <v>377</v>
@@ -28177,8 +28225,8 @@
       <c r="BK107" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL107" s="65" t="s">
-        <v>130</v>
+      <c r="BL107" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM107" s="16">
         <v>43916</v>
@@ -28189,8 +28237,8 @@
       <c r="BO107" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP107" s="1" t="s">
-        <v>130</v>
+      <c r="BP107" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ107" s="14" t="s">
         <v>377</v>
@@ -28409,8 +28457,8 @@
       <c r="BK108" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL108" s="65" t="s">
-        <v>130</v>
+      <c r="BL108" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM108" s="16">
         <v>43916</v>
@@ -28421,8 +28469,8 @@
       <c r="BO108" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP108" s="1" t="s">
-        <v>130</v>
+      <c r="BP108" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ108" s="14" t="s">
         <v>377</v>
@@ -28641,8 +28689,8 @@
       <c r="BK109" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL109" s="65" t="s">
-        <v>130</v>
+      <c r="BL109" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM109" s="16">
         <v>43916</v>
@@ -28653,8 +28701,8 @@
       <c r="BO109" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP109" s="1" t="s">
-        <v>130</v>
+      <c r="BP109" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ109" s="14" t="s">
         <v>377</v>
@@ -28873,8 +28921,8 @@
       <c r="BK110" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL110" s="4" t="s">
-        <v>130</v>
+      <c r="BL110" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM110" s="16">
         <v>43916</v>
@@ -28885,8 +28933,8 @@
       <c r="BO110" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP110" s="1" t="s">
-        <v>130</v>
+      <c r="BP110" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ110" s="14" t="s">
         <v>377</v>
@@ -29105,8 +29153,8 @@
       <c r="BK111" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL111" s="4" t="s">
-        <v>130</v>
+      <c r="BL111" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM111" s="16">
         <v>43916</v>
@@ -29117,8 +29165,8 @@
       <c r="BO111" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP111" s="1" t="s">
-        <v>130</v>
+      <c r="BP111" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ111" s="14" t="s">
         <v>377</v>
@@ -29337,8 +29385,8 @@
       <c r="BK112" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL112" s="4" t="s">
-        <v>130</v>
+      <c r="BL112" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM112" s="16">
         <v>43916</v>
@@ -29349,8 +29397,8 @@
       <c r="BO112" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP112" s="1" t="s">
-        <v>130</v>
+      <c r="BP112" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ112" s="14" t="s">
         <v>377</v>
@@ -29569,8 +29617,8 @@
       <c r="BK113" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL113" s="4" t="s">
-        <v>130</v>
+      <c r="BL113" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM113" s="16">
         <v>43916</v>
@@ -29581,8 +29629,8 @@
       <c r="BO113" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP113" s="1" t="s">
-        <v>130</v>
+      <c r="BP113" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ113" s="14" t="s">
         <v>377</v>
@@ -29784,8 +29832,8 @@
       <c r="BK114" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL114" s="4" t="s">
-        <v>130</v>
+      <c r="BL114" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM114" s="16">
         <v>43916</v>
@@ -29796,8 +29844,8 @@
       <c r="BO114" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP114" s="1" t="s">
-        <v>130</v>
+      <c r="BP114" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ114" s="14" t="s">
         <v>377</v>
@@ -29999,8 +30047,8 @@
       <c r="BK115" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL115" s="4" t="s">
-        <v>130</v>
+      <c r="BL115" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM115" s="16">
         <v>43916</v>
@@ -30011,8 +30059,8 @@
       <c r="BO115" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP115" s="1" t="s">
-        <v>130</v>
+      <c r="BP115" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ115" s="14" t="s">
         <v>377</v>
@@ -30214,8 +30262,8 @@
       <c r="BK116" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL116" s="4" t="s">
-        <v>130</v>
+      <c r="BL116" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM116" s="16">
         <v>43916</v>
@@ -30226,8 +30274,8 @@
       <c r="BO116" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP116" s="1" t="s">
-        <v>130</v>
+      <c r="BP116" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ116" s="14" t="s">
         <v>377</v>
@@ -30429,8 +30477,8 @@
       <c r="BK117" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL117" s="4" t="s">
-        <v>130</v>
+      <c r="BL117" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM117" s="16">
         <v>43916</v>
@@ -30441,8 +30489,8 @@
       <c r="BO117" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP117" s="1" t="s">
-        <v>130</v>
+      <c r="BP117" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ117" s="14" t="s">
         <v>377</v>
@@ -30644,8 +30692,8 @@
       <c r="BK118" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL118" s="4" t="s">
-        <v>130</v>
+      <c r="BL118" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM118" s="16">
         <v>43916</v>
@@ -30656,8 +30704,8 @@
       <c r="BO118" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP118" s="1" t="s">
-        <v>130</v>
+      <c r="BP118" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ118" s="14" t="s">
         <v>377</v>
@@ -30859,8 +30907,8 @@
       <c r="BK119" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL119" s="4" t="s">
-        <v>130</v>
+      <c r="BL119" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM119" s="16">
         <v>43916</v>
@@ -30871,8 +30919,8 @@
       <c r="BO119" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP119" s="1" t="s">
-        <v>130</v>
+      <c r="BP119" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ119" s="14" t="s">
         <v>377</v>
@@ -31074,8 +31122,8 @@
       <c r="BK120" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL120" s="65" t="s">
-        <v>130</v>
+      <c r="BL120" s="101" t="s">
+        <v>748</v>
       </c>
       <c r="BM120" s="16">
         <v>43916</v>
@@ -31086,8 +31134,8 @@
       <c r="BO120" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP120" s="1" t="s">
-        <v>130</v>
+      <c r="BP120" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ120" s="14" t="s">
         <v>377</v>
@@ -31289,8 +31337,8 @@
       <c r="BK121" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL121" s="65" t="s">
-        <v>130</v>
+      <c r="BL121" s="101" t="s">
+        <v>749</v>
       </c>
       <c r="BM121" s="16">
         <v>43916</v>
@@ -31301,8 +31349,8 @@
       <c r="BO121" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP121" s="1" t="s">
-        <v>130</v>
+      <c r="BP121" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ121" s="14" t="s">
         <v>377</v>
@@ -31504,8 +31552,8 @@
       <c r="BK122" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL122" s="65" t="s">
-        <v>130</v>
+      <c r="BL122" s="101" t="s">
+        <v>748</v>
       </c>
       <c r="BM122" s="16">
         <v>43916</v>
@@ -31516,8 +31564,8 @@
       <c r="BO122" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP122" s="1" t="s">
-        <v>130</v>
+      <c r="BP122" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ122" s="14" t="s">
         <v>377</v>
@@ -31719,8 +31767,8 @@
       <c r="BK123" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL123" s="65" t="s">
-        <v>130</v>
+      <c r="BL123" s="101" t="s">
+        <v>748</v>
       </c>
       <c r="BM123" s="16">
         <v>43916</v>
@@ -31731,8 +31779,8 @@
       <c r="BO123" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP123" s="1" t="s">
-        <v>130</v>
+      <c r="BP123" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ123" s="14" t="s">
         <v>377</v>
@@ -31934,8 +31982,8 @@
       <c r="BK124" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL124" s="65" t="s">
-        <v>130</v>
+      <c r="BL124" s="101" t="s">
+        <v>748</v>
       </c>
       <c r="BM124" s="16">
         <v>43916</v>
@@ -31946,8 +31994,8 @@
       <c r="BO124" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP124" s="1" t="s">
-        <v>130</v>
+      <c r="BP124" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ124" s="14" t="s">
         <v>377</v>
@@ -32149,8 +32197,8 @@
       <c r="BK125" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL125" s="65" t="s">
-        <v>130</v>
+      <c r="BL125" s="101" t="s">
+        <v>750</v>
       </c>
       <c r="BM125" s="16">
         <v>43916</v>
@@ -32161,8 +32209,8 @@
       <c r="BO125" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP125" s="1" t="s">
-        <v>130</v>
+      <c r="BP125" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ125" s="14" t="s">
         <v>377</v>
@@ -32364,8 +32412,8 @@
       <c r="BK126" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL126" s="65" t="s">
-        <v>130</v>
+      <c r="BL126" s="101" t="s">
+        <v>751</v>
       </c>
       <c r="BM126" s="16">
         <v>43916</v>
@@ -32376,8 +32424,8 @@
       <c r="BO126" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP126" s="1" t="s">
-        <v>130</v>
+      <c r="BP126" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ126" s="14" t="s">
         <v>377</v>
@@ -32579,8 +32627,8 @@
       <c r="BK127" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL127" s="65" t="s">
-        <v>130</v>
+      <c r="BL127" s="101" t="s">
+        <v>749</v>
       </c>
       <c r="BM127" s="16">
         <v>43916</v>
@@ -32591,8 +32639,8 @@
       <c r="BO127" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP127" s="1" t="s">
-        <v>130</v>
+      <c r="BP127" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ127" s="14" t="s">
         <v>377</v>
@@ -32794,8 +32842,8 @@
       <c r="BK128" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL128" s="65" t="s">
-        <v>130</v>
+      <c r="BL128" s="101" t="s">
+        <v>749</v>
       </c>
       <c r="BM128" s="16">
         <v>43916</v>
@@ -32806,8 +32854,8 @@
       <c r="BO128" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP128" s="1" t="s">
-        <v>130</v>
+      <c r="BP128" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ128" s="14" t="s">
         <v>377</v>
@@ -33009,8 +33057,8 @@
       <c r="BK129" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL129" s="65" t="s">
-        <v>130</v>
+      <c r="BL129" s="101" t="s">
+        <v>749</v>
       </c>
       <c r="BM129" s="16">
         <v>43916</v>
@@ -33021,8 +33069,8 @@
       <c r="BO129" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP129" s="1" t="s">
-        <v>130</v>
+      <c r="BP129" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ129" s="14" t="s">
         <v>377</v>
@@ -33224,8 +33272,8 @@
       <c r="BK130" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL130" s="65" t="s">
-        <v>130</v>
+      <c r="BL130" s="101" t="s">
+        <v>749</v>
       </c>
       <c r="BM130" s="16">
         <v>43916</v>
@@ -33236,8 +33284,8 @@
       <c r="BO130" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP130" s="1" t="s">
-        <v>130</v>
+      <c r="BP130" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ130" s="14" t="s">
         <v>377</v>
@@ -33439,8 +33487,8 @@
       <c r="BK131" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL131" s="65" t="s">
-        <v>130</v>
+      <c r="BL131" s="101" t="s">
+        <v>752</v>
       </c>
       <c r="BM131" s="16">
         <v>43916</v>
@@ -33451,8 +33499,8 @@
       <c r="BO131" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP131" s="1" t="s">
-        <v>130</v>
+      <c r="BP131" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ131" s="14" t="s">
         <v>377</v>
@@ -33654,8 +33702,8 @@
       <c r="BK132" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL132" s="65" t="s">
-        <v>130</v>
+      <c r="BL132" s="101" t="s">
+        <v>751</v>
       </c>
       <c r="BM132" s="16">
         <v>43916</v>
@@ -33666,8 +33714,8 @@
       <c r="BO132" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP132" s="1" t="s">
-        <v>130</v>
+      <c r="BP132" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ132" s="14" t="s">
         <v>377</v>
@@ -33869,8 +33917,8 @@
       <c r="BK133" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL133" s="65" t="s">
-        <v>130</v>
+      <c r="BL133" s="101" t="s">
+        <v>752</v>
       </c>
       <c r="BM133" s="16">
         <v>43916</v>
@@ -33881,8 +33929,8 @@
       <c r="BO133" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP133" s="1" t="s">
-        <v>130</v>
+      <c r="BP133" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ133" s="14" t="s">
         <v>377</v>
@@ -34084,8 +34132,8 @@
       <c r="BK134" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL134" s="65" t="s">
-        <v>130</v>
+      <c r="BL134" s="101" t="s">
+        <v>749</v>
       </c>
       <c r="BM134" s="16">
         <v>43916</v>
@@ -34096,8 +34144,8 @@
       <c r="BO134" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP134" s="1" t="s">
-        <v>130</v>
+      <c r="BP134" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ134" s="14" t="s">
         <v>377</v>
@@ -34299,8 +34347,8 @@
       <c r="BK135" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL135" s="65" t="s">
-        <v>130</v>
+      <c r="BL135" s="101" t="s">
+        <v>753</v>
       </c>
       <c r="BM135" s="16">
         <v>43916</v>
@@ -34311,8 +34359,8 @@
       <c r="BO135" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP135" s="1" t="s">
-        <v>130</v>
+      <c r="BP135" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ135" s="14" t="s">
         <v>377</v>
@@ -34514,8 +34562,8 @@
       <c r="BK136" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL136" s="65" t="s">
-        <v>130</v>
+      <c r="BL136" s="101" t="s">
+        <v>753</v>
       </c>
       <c r="BM136" s="16">
         <v>43916</v>
@@ -34526,8 +34574,8 @@
       <c r="BO136" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP136" s="1" t="s">
-        <v>130</v>
+      <c r="BP136" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ136" s="14" t="s">
         <v>377</v>
@@ -34729,8 +34777,8 @@
       <c r="BK137" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL137" s="65" t="s">
-        <v>130</v>
+      <c r="BL137" s="101" t="s">
+        <v>753</v>
       </c>
       <c r="BM137" s="16">
         <v>43916</v>
@@ -34741,8 +34789,8 @@
       <c r="BO137" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP137" s="1" t="s">
-        <v>130</v>
+      <c r="BP137" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ137" s="14" t="s">
         <v>377</v>
@@ -34944,8 +34992,8 @@
       <c r="BK138" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL138" s="65" t="s">
-        <v>130</v>
+      <c r="BL138" s="101" t="s">
+        <v>751</v>
       </c>
       <c r="BM138" s="16">
         <v>43916</v>
@@ -34956,8 +35004,8 @@
       <c r="BO138" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP138" s="1" t="s">
-        <v>130</v>
+      <c r="BP138" s="101" t="s">
+        <v>744</v>
       </c>
       <c r="BQ138" s="14" t="s">
         <v>377</v>
@@ -35159,8 +35207,8 @@
       <c r="BK139" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL139" s="65" t="s">
-        <v>130</v>
+      <c r="BL139" s="101" t="s">
+        <v>754</v>
       </c>
       <c r="BM139" s="16">
         <v>43916</v>
@@ -35171,8 +35219,8 @@
       <c r="BO139" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP139" s="1" t="s">
-        <v>130</v>
+      <c r="BP139" s="101" t="s">
+        <v>746</v>
       </c>
       <c r="BQ139" s="14" t="s">
         <v>377</v>
@@ -35374,8 +35422,8 @@
       <c r="BK140" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL140" s="65" t="s">
-        <v>130</v>
+      <c r="BL140" s="101" t="s">
+        <v>749</v>
       </c>
       <c r="BM140" s="16">
         <v>43916</v>
@@ -35386,8 +35434,8 @@
       <c r="BO140" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP140" s="1" t="s">
-        <v>130</v>
+      <c r="BP140" s="101" t="s">
+        <v>746</v>
       </c>
       <c r="BQ140" s="14" t="s">
         <v>377</v>
@@ -35589,8 +35637,8 @@
       <c r="BK141" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL141" s="65" t="s">
-        <v>130</v>
+      <c r="BL141" s="101" t="s">
+        <v>754</v>
       </c>
       <c r="BM141" s="16">
         <v>43916</v>
@@ -35601,8 +35649,8 @@
       <c r="BO141" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP141" s="1" t="s">
-        <v>130</v>
+      <c r="BP141" s="101" t="s">
+        <v>746</v>
       </c>
       <c r="BQ141" s="14" t="s">
         <v>377</v>
@@ -35804,8 +35852,8 @@
       <c r="BK142" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL142" s="65" t="s">
-        <v>130</v>
+      <c r="BL142" s="101" t="s">
+        <v>755</v>
       </c>
       <c r="BM142" s="16">
         <v>43916</v>
@@ -35816,8 +35864,8 @@
       <c r="BO142" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP142" s="1" t="s">
-        <v>130</v>
+      <c r="BP142" s="101" t="s">
+        <v>746</v>
       </c>
       <c r="BQ142" s="14" t="s">
         <v>377</v>
@@ -36019,8 +36067,8 @@
       <c r="BK143" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL143" s="65" t="s">
-        <v>130</v>
+      <c r="BL143" s="101" t="s">
+        <v>756</v>
       </c>
       <c r="BM143" s="16">
         <v>43916</v>
@@ -36031,8 +36079,8 @@
       <c r="BO143" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP143" s="1" t="s">
-        <v>130</v>
+      <c r="BP143" s="101" t="s">
+        <v>746</v>
       </c>
       <c r="BQ143" s="14" t="s">
         <v>377</v>
@@ -36234,8 +36282,8 @@
       <c r="BK144" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL144" s="65" t="s">
-        <v>130</v>
+      <c r="BL144" s="101" t="s">
+        <v>757</v>
       </c>
       <c r="BM144" s="16">
         <v>43916</v>
@@ -36246,8 +36294,8 @@
       <c r="BO144" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="BP144" s="1" t="s">
-        <v>130</v>
+      <c r="BP144" s="101" t="s">
+        <v>746</v>
       </c>
       <c r="BQ144" s="14" t="s">
         <v>377</v>
@@ -36449,8 +36497,8 @@
       <c r="BK145" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL145" s="65" t="s">
-        <v>130</v>
+      <c r="BL145" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM145" s="65" t="s">
         <v>130</v>
@@ -36461,8 +36509,8 @@
       <c r="BO145" s="65" t="s">
         <v>130</v>
       </c>
-      <c r="BP145" s="1" t="s">
-        <v>130</v>
+      <c r="BP145" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ145" s="1" t="s">
         <v>130</v>
@@ -36664,8 +36712,8 @@
       <c r="BK146" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL146" s="65" t="s">
-        <v>130</v>
+      <c r="BL146" s="101" t="s">
+        <v>747</v>
       </c>
       <c r="BM146" s="65" t="s">
         <v>130</v>
@@ -36676,8 +36724,8 @@
       <c r="BO146" s="65" t="s">
         <v>130</v>
       </c>
-      <c r="BP146" s="1" t="s">
-        <v>130</v>
+      <c r="BP146" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ146" s="1" t="s">
         <v>130</v>
@@ -36879,8 +36927,8 @@
       <c r="BK147" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL147" s="65" t="s">
-        <v>130</v>
+      <c r="BL147" s="101" t="s">
+        <v>758</v>
       </c>
       <c r="BM147" s="65" t="s">
         <v>130</v>
@@ -36891,8 +36939,8 @@
       <c r="BO147" s="65" t="s">
         <v>130</v>
       </c>
-      <c r="BP147" s="1" t="s">
-        <v>130</v>
+      <c r="BP147" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ147" s="1" t="s">
         <v>130</v>
@@ -37094,8 +37142,8 @@
       <c r="BK148" s="49" t="s">
         <v>130</v>
       </c>
-      <c r="BL148" s="65" t="s">
-        <v>130</v>
+      <c r="BL148" s="101" t="s">
+        <v>758</v>
       </c>
       <c r="BM148" s="65" t="s">
         <v>130</v>
@@ -37106,8 +37154,8 @@
       <c r="BO148" s="65" t="s">
         <v>130</v>
       </c>
-      <c r="BP148" s="1" t="s">
-        <v>130</v>
+      <c r="BP148" s="101" t="s">
+        <v>745</v>
       </c>
       <c r="BQ148" s="1" t="s">
         <v>130</v>

</xml_diff>